<commit_message>
egyeni jelentes and projektterv update
</commit_message>
<xml_diff>
--- a/Gantt_diagram_etel.xlsx
+++ b/Gantt_diagram_etel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kriszti\2024_ib153l-15_etel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E8B047-A670-47A9-A35F-B4358F735F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ACBF80-E22B-4D2A-8BBC-1689EF1B8875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt-diagram" sheetId="1" r:id="rId1"/>
@@ -886,163 +886,7 @@
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-      </border>
-    </dxf>
+  <dxfs count="34">
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -1701,9 +1545,9 @@
   </sheetPr>
   <dimension ref="A1:CL1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CK41" sqref="CK41:CL41"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" activeCellId="1" sqref="C26 C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5244,7 +5088,7 @@
         <v>45</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D36" s="59">
         <v>45598</v>
@@ -5300,7 +5144,7 @@
       <c r="AY36" s="30"/>
       <c r="AZ36" s="30"/>
       <c r="BA36" s="30"/>
-      <c r="BB36" s="52"/>
+      <c r="BB36" s="51"/>
       <c r="BC36" s="38"/>
       <c r="BD36" s="30"/>
       <c r="BE36" s="30"/>
@@ -5344,7 +5188,7 @@
         <v>46</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D37" s="59">
         <v>45598</v>
@@ -5400,8 +5244,8 @@
       <c r="AY37" s="30"/>
       <c r="AZ37" s="30"/>
       <c r="BA37" s="30"/>
-      <c r="BB37" s="52"/>
-      <c r="BC37" s="52"/>
+      <c r="BB37" s="51"/>
+      <c r="BC37" s="51"/>
       <c r="BD37" s="30"/>
       <c r="BE37" s="30"/>
       <c r="BF37" s="30"/>
@@ -6442,7 +6286,7 @@
         <v>56</v>
       </c>
       <c r="C48" s="69" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D48" s="70">
         <v>45615</v>
@@ -6515,7 +6359,7 @@
       <c r="BP48" s="38"/>
       <c r="BQ48" s="38"/>
       <c r="BR48" s="30"/>
-      <c r="BS48" s="47"/>
+      <c r="BS48" s="40"/>
       <c r="BT48" s="30"/>
       <c r="BU48" s="30"/>
       <c r="BV48" s="30"/>
@@ -6542,7 +6386,7 @@
         <v>57</v>
       </c>
       <c r="C49" s="69" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D49" s="70">
         <v>45614</v>
@@ -6614,7 +6458,7 @@
       <c r="BO49" s="30"/>
       <c r="BP49" s="38"/>
       <c r="BQ49" s="38"/>
-      <c r="BR49" s="47"/>
+      <c r="BR49" s="40"/>
       <c r="BS49" s="30"/>
       <c r="BT49" s="30"/>
       <c r="BU49" s="30"/>
@@ -11982,234 +11826,174 @@
     <mergeCell ref="BD4:BJ4"/>
     <mergeCell ref="BK4:BQ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="BD43:CC52 BD53:BQ53 BT53:CC53 BD54:CC54 G8:T40 G42:T42 AN32:AT40 G43:AT54 AW40:BA40 AU42:BA54 CD8:CE40 CD42:CE54 AG11:AM40 AB18:AF40 AB42:AT42 AU20:AV40 CK19:CL40 CK42:CL54">
-    <cfRule type="expression" dxfId="45" priority="31">
+  <conditionalFormatting sqref="G8:T41">
+    <cfRule type="expression" dxfId="33" priority="25">
       <formula>AND(TODAY()&gt;=G$5,TODAY()&lt;H$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:BW6 BY6:CD6 U8:W8 AG8:AT10 AB17:AE17 AP19:AT33 AZ23:BA31 AW24:AW28 AX24:AY31 AW30:AW32 AY34:BA35 AW36:AW38 AX38:AZ38 CF42:CL42">
-    <cfRule type="expression" dxfId="44" priority="32">
+    <cfRule type="expression" dxfId="32" priority="34">
       <formula>AND(TODAY()&gt;=G$5,TODAY()&lt;H$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U8:Y17 Z8:AA40">
-    <cfRule type="expression" dxfId="43" priority="33">
+  <conditionalFormatting sqref="U8:Y17">
+    <cfRule type="expression" dxfId="31" priority="35">
       <formula>AND(TODAY()&gt;=U$5,TODAY()&lt;V$5)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="U16:Y41">
+    <cfRule type="expression" dxfId="30" priority="23">
+      <formula>AND(TODAY()&gt;=BD$5,TODAY()&lt;BE$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="V11:X11">
-    <cfRule type="expression" dxfId="42" priority="34">
+    <cfRule type="expression" dxfId="29" priority="36">
       <formula>AND(TODAY()&gt;=V$5,TODAY()&lt;W$5)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="Z8:AA41">
+    <cfRule type="expression" dxfId="28" priority="22">
+      <formula>AND(TODAY()&gt;=Z$5,TODAY()&lt;AA$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AB8:AF16">
-    <cfRule type="expression" dxfId="41" priority="37">
+    <cfRule type="expression" dxfId="27" priority="39">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;AC$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U42:AA42">
-    <cfRule type="expression" dxfId="40" priority="38">
-      <formula>AND(TODAY()&gt;=U$5,TODAY()&lt;V$5)</formula>
+  <conditionalFormatting sqref="AB18:AF41">
+    <cfRule type="expression" dxfId="26" priority="21">
+      <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;AC$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG11:AM40 AN32:AT40 G42:BA54 BD53:BQ53 BT53:CC53 BD54:CC54 BD43:CC52">
+    <cfRule type="expression" dxfId="25" priority="33">
+      <formula>AND(TODAY()&gt;=G$5,TODAY()&lt;H$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG41:AT41">
+    <cfRule type="expression" dxfId="24" priority="17">
+      <formula>AND(TODAY()&gt;=AG$5,TODAY()&lt;AH$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN11:AT17 AN18:BO18 AN19:AO31">
-    <cfRule type="expression" dxfId="39" priority="40">
+    <cfRule type="expression" dxfId="23" priority="42">
       <formula>AND(TODAY()&gt;=AN$5,TODAY()&lt;AO$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT26:AV28">
-    <cfRule type="expression" dxfId="38" priority="41">
+    <cfRule type="expression" dxfId="22" priority="43">
       <formula>AND(TODAY()&gt;=AT$5,TODAY()&lt;AU$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AU8:BC17 AU19:BC21 AW20:BC40">
-    <cfRule type="expression" dxfId="37" priority="43">
+  <conditionalFormatting sqref="AU20:AV41">
+    <cfRule type="expression" dxfId="21" priority="16">
       <formula>AND(TODAY()&gt;=AU$5,TODAY()&lt;AV$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BB42:BC54">
-    <cfRule type="expression" dxfId="36" priority="44">
+  <conditionalFormatting sqref="AU8:BC17 AU19:BC21 AW20:BC35 AW38:BC40 BC36 AW36:BA37">
+    <cfRule type="expression" dxfId="20" priority="45">
+      <formula>AND(TODAY()&gt;=AU$5,TODAY()&lt;AV$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW40:BA41">
+    <cfRule type="expression" dxfId="19" priority="14">
+      <formula>AND(TODAY()&gt;=AW$5,TODAY()&lt;AX$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB41:BC54">
+    <cfRule type="expression" dxfId="18" priority="13">
       <formula>AND(TODAY()&gt;=BB$5,TODAY()&lt;BC$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BD8:BO17 U16:Y40 BH19:BJ26 BT53:BT54 BP8:CC40 BD19:BG40 BK19:BO40 BH28:BJ40 BD42:CC42">
-    <cfRule type="expression" dxfId="35" priority="45">
-      <formula>AND(TODAY()&gt;=BD$5,TODAY()&lt;BE$5)</formula>
+  <conditionalFormatting sqref="BD19:BG41">
+    <cfRule type="expression" dxfId="17" priority="12">
+      <formula>AND(TODAY()&gt;=CM$5,TODAY()&lt;CN$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BD8:BO17 BH19:BJ26 BD42:CC42 BT53:BT54">
+    <cfRule type="expression" dxfId="16" priority="47">
+      <formula>AND(TODAY()&gt;=CM$5,TODAY()&lt;CN$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BH28:BJ41">
+    <cfRule type="expression" dxfId="15" priority="10">
+      <formula>AND(TODAY()&gt;=CQ$5,TODAY()&lt;CR$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BK19:BO41">
+    <cfRule type="expression" dxfId="14" priority="11">
+      <formula>AND(TODAY()&gt;=CT$5,TODAY()&lt;CU$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BP8:CC41">
+    <cfRule type="expression" dxfId="13" priority="6">
+      <formula>AND(TODAY()&gt;=CY$5,TODAY()&lt;CZ$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR53:BS53">
-    <cfRule type="expression" dxfId="34" priority="27">
+    <cfRule type="expression" dxfId="12" priority="29">
       <formula>AND(TODAY()&gt;=DA$5,TODAY()&lt;DB$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BU54:BV54">
-    <cfRule type="expression" dxfId="33" priority="30">
+    <cfRule type="expression" dxfId="11" priority="32">
       <formula>AND(TODAY()&gt;=DD$5,TODAY()&lt;DE$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BX5">
-    <cfRule type="expression" dxfId="32" priority="46">
+    <cfRule type="expression" dxfId="10" priority="48">
       <formula>AND(TODAY()&gt;=BX$5,TODAY()&lt;BY$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BY5:CD5 CF5:CK5 BX6 CE6">
-    <cfRule type="expression" dxfId="31" priority="47">
+    <cfRule type="expression" dxfId="9" priority="49">
       <formula>AND(TODAY()&gt;=BX$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="CD8:CE54">
+    <cfRule type="expression" dxfId="8" priority="5">
+      <formula>AND(TODAY()&gt;=CD$5,TODAY()&lt;CE$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="CE5">
-    <cfRule type="expression" dxfId="30" priority="48">
+    <cfRule type="expression" dxfId="7" priority="50">
       <formula>AND(TODAY()&gt;=CE$5,TODAY()&lt;CF$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CF19:CJ40">
-    <cfRule type="expression" dxfId="29" priority="49">
+  <conditionalFormatting sqref="CF19:CJ41">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>AND(TODAY()&gt;=CF$5,TODAY()&lt;CG$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CF43:CJ54">
-    <cfRule type="expression" dxfId="28" priority="29">
+    <cfRule type="expression" dxfId="5" priority="31">
       <formula>AND(TODAY()&gt;=CF$5,TODAY()&lt;CG$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CF8:CL18">
-    <cfRule type="expression" dxfId="27" priority="51">
+    <cfRule type="expression" dxfId="4" priority="53">
       <formula>AND(TODAY()&gt;=CF$5,TODAY()&lt;CG$5)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="CK19:CL54">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>AND(TODAY()&gt;=CK$5,TODAY()&lt;CL$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="CL5">
-    <cfRule type="expression" dxfId="26" priority="54">
+    <cfRule type="expression" dxfId="2" priority="56">
       <formula>AND(TODAY()&gt;=CL$5,TODAY()&lt;CM$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G41:K41">
-    <cfRule type="expression" dxfId="25" priority="26">
-      <formula>AND(TODAY()&gt;=G$5,TODAY()&lt;H$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L41:M41">
-    <cfRule type="expression" dxfId="24" priority="25">
-      <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N41:R41">
-    <cfRule type="expression" dxfId="23" priority="24">
-      <formula>AND(TODAY()&gt;=N$5,TODAY()&lt;O$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S41:T41">
-    <cfRule type="expression" dxfId="22" priority="23">
-      <formula>AND(TODAY()&gt;=S$5,TODAY()&lt;T$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BH41:BI41">
-    <cfRule type="expression" dxfId="21" priority="22">
-      <formula>AND(TODAY()&gt;=CQ$5,TODAY()&lt;CR$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U41:Y41">
-    <cfRule type="expression" dxfId="20" priority="21">
-      <formula>AND(TODAY()&gt;=BD$5,TODAY()&lt;BE$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z41:AA41">
-    <cfRule type="expression" dxfId="19" priority="20">
-      <formula>AND(TODAY()&gt;=Z$5,TODAY()&lt;AA$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB41:AF41">
-    <cfRule type="expression" dxfId="18" priority="19">
-      <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;AC$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG41:AH41">
-    <cfRule type="expression" dxfId="17" priority="18">
-      <formula>AND(TODAY()&gt;=AG$5,TODAY()&lt;AH$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI41:AM41">
-    <cfRule type="expression" dxfId="16" priority="17">
-      <formula>AND(TODAY()&gt;=AI$5,TODAY()&lt;AJ$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN41:AO41">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>AND(TODAY()&gt;=AN$5,TODAY()&lt;AO$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP41:AT41">
-    <cfRule type="expression" dxfId="14" priority="15">
-      <formula>AND(TODAY()&gt;=AP$5,TODAY()&lt;AQ$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AU41:AV41">
-    <cfRule type="expression" dxfId="13" priority="14">
-      <formula>AND(TODAY()&gt;=AU$5,TODAY()&lt;AV$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AW41:BA41">
-    <cfRule type="expression" dxfId="12" priority="12">
-      <formula>AND(TODAY()&gt;=AW$5,TODAY()&lt;AX$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AW41:BA41">
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>AND(TODAY()&gt;=AW$5,TODAY()&lt;AX$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BB41:BC41">
-    <cfRule type="expression" dxfId="10" priority="11">
+  <conditionalFormatting sqref="BB36">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(TODAY()&gt;=BB$5,TODAY()&lt;BC$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BD41:BG41">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>AND(TODAY()&gt;=CM$5,TODAY()&lt;CN$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BK41:BO41">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>AND(TODAY()&gt;=CT$5,TODAY()&lt;CU$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BJ41">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>AND(TODAY()&gt;=CS$5,TODAY()&lt;CT$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BP41:BQ41">
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>AND(TODAY()&gt;=CY$5,TODAY()&lt;CZ$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BR41:BV41">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>AND(TODAY()&gt;=DA$5,TODAY()&lt;DB$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BW41:BX41">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>AND(TODAY()&gt;=DF$5,TODAY()&lt;DG$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BY41:CC41">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>AND(TODAY()&gt;=DH$5,TODAY()&lt;DI$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CD41:CE41">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>AND(TODAY()&gt;=CD$5,TODAY()&lt;CE$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CF41:CJ41">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>AND(TODAY()&gt;=CF$5,TODAY()&lt;CG$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CK41:CL41">
+  <conditionalFormatting sqref="BB37:BC37">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(TODAY()&gt;=CK$5,TODAY()&lt;CL$5)</formula>
+      <formula>AND(TODAY()&gt;=BB$5,TODAY()&lt;BC$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>

</xml_diff>